<commit_message>
upadting final excel files
</commit_message>
<xml_diff>
--- a/doc/Models.xlsx
+++ b/doc/Models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDriveMirror\UNI\Thesis\Files\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917CA728-95BC-4BEE-B9E4-C41FD33A0F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A604799-625F-4A0A-BF1C-494D74397E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Models</t>
   </si>
@@ -65,16 +65,10 @@
     <t>Qwen2 1.5B</t>
   </si>
   <si>
-    <t>Llama 3.2 1B</t>
-  </si>
-  <si>
     <t>Phi 2</t>
   </si>
   <si>
     <t>Qwen2.5 3B</t>
-  </si>
-  <si>
-    <t>Llama 3.2m 3B</t>
   </si>
   <si>
     <t>Qwen 1.5 4B</t>
@@ -448,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="E22" sqref="E21:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +460,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -478,7 +472,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
@@ -507,7 +501,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <f t="shared" ref="A3:A18" si="0">ROW()-1</f>
+        <f t="shared" ref="A3:A16" si="0">ROW()-1</f>
         <v>2</v>
       </c>
       <c r="B3" s="3">
@@ -532,16 +526,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>4421</v>
+        <v>3438</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3">
-        <v>1.24</v>
+        <v>1.5</v>
       </c>
       <c r="E4" s="3">
-        <v>4.2</v>
+        <v>13.85</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>2</v>
@@ -553,16 +547,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>3438</v>
+        <v>3703</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="3">
-        <v>1.5</v>
+        <v>1.544</v>
       </c>
       <c r="E5" s="3">
-        <v>13.85</v>
+        <v>10.45</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>2</v>
@@ -574,16 +568,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <v>3703</v>
+        <v>3250</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3">
-        <v>1.544</v>
+        <v>2.78</v>
       </c>
       <c r="E6" s="3">
-        <v>10.45</v>
+        <v>15.53</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>2</v>
@@ -595,16 +589,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>3250</v>
+        <v>3619</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3">
-        <v>2.78</v>
+        <v>2.85</v>
       </c>
       <c r="E7" s="3">
-        <v>15.53</v>
+        <v>11.71</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>2</v>
@@ -616,16 +610,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>3619</v>
+        <v>2940</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3">
-        <v>2.85</v>
+        <v>3.0859999999999999</v>
       </c>
       <c r="E8" s="3">
-        <v>11.71</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>2</v>
@@ -637,16 +631,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>2940</v>
+        <v>3616</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="3">
-        <v>3.0859999999999999</v>
+        <v>3.95</v>
       </c>
       <c r="E9" s="3">
-        <v>18.100000000000001</v>
+        <v>11.77</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>2</v>
@@ -658,16 +652,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>3809</v>
+        <v>3096</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D10" s="3">
-        <v>3.2130000000000001</v>
+        <v>6.0609999999999999</v>
       </c>
       <c r="E10" s="3">
-        <v>8.6999999999999993</v>
+        <v>16.75</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>2</v>
@@ -679,16 +673,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="3">
-        <v>3616</v>
+        <v>3008</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="3">
-        <v>3.95</v>
+        <v>6.9189999999999996</v>
       </c>
       <c r="E11" s="3">
-        <v>11.77</v>
+        <v>17.510000000000002</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>2</v>
@@ -700,16 +694,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="3">
-        <v>3096</v>
+        <v>1502</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="3">
-        <v>6.0609999999999999</v>
+        <v>7.6159999999999997</v>
       </c>
       <c r="E12" s="3">
-        <v>16.75</v>
+        <v>26.02</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>2</v>
@@ -721,16 +715,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="3">
-        <v>3008</v>
+        <v>1862</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" s="3">
-        <v>6.9189999999999996</v>
+        <v>7.6159999999999997</v>
       </c>
       <c r="E13" s="3">
-        <v>17.510000000000002</v>
+        <v>23.93</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>2</v>
@@ -742,16 +736,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="3">
-        <v>1502</v>
+        <v>1905</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="3">
-        <v>7.6159999999999997</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="E14" s="3">
-        <v>26.02</v>
+        <v>23.76</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>2</v>
@@ -763,16 +757,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="3">
-        <v>1862</v>
+        <v>2256</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="3">
-        <v>7.6159999999999997</v>
+        <v>8.8290000000000006</v>
       </c>
       <c r="E15" s="3">
-        <v>23.93</v>
+        <v>22.15</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>2</v>
@@ -784,60 +778,18 @@
         <v>15</v>
       </c>
       <c r="B16" s="3">
-        <v>1905</v>
+        <v>2456</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="3">
-        <v>8.0299999999999994</v>
+        <v>9</v>
       </c>
       <c r="E16" s="3">
-        <v>23.76</v>
+        <v>21.21</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="3">
-        <v>2256</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="3">
-        <v>8.8290000000000006</v>
-      </c>
-      <c r="E17" s="3">
-        <v>22.15</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="3">
-        <v>2456</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="3">
-        <v>9</v>
-      </c>
-      <c r="E18" s="3">
-        <v>21.21</v>
-      </c>
-      <c r="F18" s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>